<commit_message>
Get_Quotes() kann nun domestic und foreign quotes runterladen
</commit_message>
<xml_diff>
--- a/FinaLytics_Template_2.xlsx
+++ b/FinaLytics_Template_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FinaLytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73C6C2E-BC36-4030-82A1-12D0544211BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0381DE19-396D-4572-9318-4A1A512C1536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14490" yWindow="-1245" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -118,12 +118,6 @@
     <t>AE5A.DE</t>
   </si>
   <si>
-    <t>FXXSC.DE</t>
-  </si>
-  <si>
-    <t>MSE.MI</t>
-  </si>
-  <si>
     <t>TMV.DE</t>
   </si>
   <si>
@@ -152,6 +146,12 @@
   </si>
   <si>
     <t>iShares Automation</t>
+  </si>
+  <si>
+    <t>MSE.PA</t>
+  </si>
+  <si>
+    <t>DX2J.F</t>
   </si>
 </sst>
 </file>
@@ -526,7 +526,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,7 +641,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -661,7 +661,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
@@ -681,7 +681,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
@@ -721,7 +721,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
         <v>20</v>
@@ -741,7 +741,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
         <v>21</v>
@@ -761,7 +761,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
         <v>22</v>
@@ -781,7 +781,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
         <v>23</v>
@@ -801,7 +801,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
         <v>24</v>
@@ -821,7 +821,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B15" t="s">
         <v>25</v>
@@ -841,7 +841,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B16" t="s">
         <v>26</v>
@@ -881,10 +881,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C18">
         <v>10.61</v>

</xml_diff>

<commit_message>
Default-Werte für width und height hinzugefügt. Bei Instanzinierung änderbar
</commit_message>
<xml_diff>
--- a/FinaLytics_Template_2.xlsx
+++ b/FinaLytics_Template_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FinaLytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0381DE19-396D-4572-9318-4A1A512C1536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A77B83-E4AD-4C34-96E5-3E83A289766B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-43050" yWindow="2550" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -112,46 +112,46 @@
     <t>MWRD.PA</t>
   </si>
   <si>
-    <t>NADQ.DE</t>
+    <t>TMV.DE</t>
+  </si>
+  <si>
+    <t>EXV9.DE</t>
+  </si>
+  <si>
+    <t>ADJ.DE</t>
+  </si>
+  <si>
+    <t>BAYN.DE</t>
+  </si>
+  <si>
+    <t>04Q.DE</t>
+  </si>
+  <si>
+    <t>TSLA</t>
+  </si>
+  <si>
+    <t>DE000A30WFV1.SG</t>
+  </si>
+  <si>
+    <t>XS2589367528.SG</t>
+  </si>
+  <si>
+    <t>RBOT.L</t>
+  </si>
+  <si>
+    <t>iShares Automation</t>
+  </si>
+  <si>
+    <t>MSE.PA</t>
+  </si>
+  <si>
+    <t>DX2J.F</t>
+  </si>
+  <si>
+    <t>NADQ.SW</t>
   </si>
   <si>
     <t>AE5A.DE</t>
-  </si>
-  <si>
-    <t>TMV.DE</t>
-  </si>
-  <si>
-    <t>EXV9.DE</t>
-  </si>
-  <si>
-    <t>ADJ.DE</t>
-  </si>
-  <si>
-    <t>BAYN.DE</t>
-  </si>
-  <si>
-    <t>04Q.DE</t>
-  </si>
-  <si>
-    <t>TSLA</t>
-  </si>
-  <si>
-    <t>DE000A30WFV1.SG</t>
-  </si>
-  <si>
-    <t>XS2589367528.SG</t>
-  </si>
-  <si>
-    <t>RBOT.L</t>
-  </si>
-  <si>
-    <t>iShares Automation</t>
-  </si>
-  <si>
-    <t>MSE.PA</t>
-  </si>
-  <si>
-    <t>DX2J.F</t>
   </si>
 </sst>
 </file>
@@ -526,7 +526,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,7 +601,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
@@ -621,7 +621,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
@@ -641,7 +641,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -661,7 +661,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
@@ -681,7 +681,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
@@ -721,7 +721,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
         <v>20</v>
@@ -741,7 +741,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
         <v>21</v>
@@ -761,7 +761,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
         <v>22</v>
@@ -781,7 +781,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
         <v>23</v>
@@ -801,7 +801,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
         <v>24</v>
@@ -821,7 +821,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
         <v>25</v>
@@ -841,7 +841,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
         <v>26</v>
@@ -881,10 +881,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C18">
         <v>10.61</v>

</xml_diff>